<commit_message>
bad and basic translation of messages
</commit_message>
<xml_diff>
--- a/tests/spreadsheets/albums.xlsx
+++ b/tests/spreadsheets/albums.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julian/Desktop/pina_bausch_online_archiv/05_Development/superspreader/tests/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB707F71-D8CA-1A4A-AD3B-A65839AB76AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90449015-21B4-5D4C-8B8F-D4F3BAE71DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{AEA88CA7-DB4E-854B-B403-00CA6CDC1E3D}"/>
+    <workbookView xWindow="-23660" yWindow="-10980" windowWidth="28800" windowHeight="17500" xr2:uid="{AEA88CA7-DB4E-854B-B403-00CA6CDC1E3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Albums" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Artist</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t>Fix Yourself, Not The World</t>
+  </si>
+  <si>
+    <t>Kokoroko</t>
+  </si>
+  <si>
+    <t>Could We Be More</t>
   </si>
 </sst>
 </file>
@@ -426,7 +432,7 @@
   <dimension ref="A2:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -492,19 +498,19 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2">
-        <v>43191</v>
+        <v>44774</v>
       </c>
       <c r="D7">
-        <v>3.9</v>
+        <v>4.7</v>
       </c>
       <c r="E7">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>